<commit_message>
raw data set from team manager database started the script to format the data, added code to create a new time schema along side of score schema
</commit_message>
<xml_diff>
--- a/data/ilikeswim.xlsx
+++ b/data/ilikeswim.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10309"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alansun/Documents/18-19/ee/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alansun/Documents/18-19/ee/app/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C259C60-8A87-B64B-9B33-69F933F426CE}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE13D7A1-B022-0748-B272-F9594C5F9B20}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28540" windowHeight="16340" xr2:uid="{138EBCB2-7A5F-2A45-8846-3DFC627D2A5A}"/>
+    <workbookView xWindow="28820" yWindow="460" windowWidth="25340" windowHeight="28340" xr2:uid="{138EBCB2-7A5F-2A45-8846-3DFC627D2A5A}"/>
   </bookViews>
   <sheets>
     <sheet name="bois" sheetId="1" r:id="rId1"/>
@@ -1259,8 +1259,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1041A3BC-6B0B-9E47-9860-052DCE494B28}">
   <dimension ref="A1:P173"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="C5" sqref="C1:C1048576"/>
+    <sheetView tabSelected="1" zoomScale="193" zoomScaleNormal="193" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5454,7 +5454,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62230908-BA10-334E-AC56-27BA51336630}">
   <dimension ref="A1:P91"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>

</xml_diff>